<commit_message>
Adjusted to include a 110kV node as well
</commit_message>
<xml_diff>
--- a/hast2_1/tests/HAST_Inputs_stage0.xlsx
+++ b/hast2_1/tests/HAST_Inputs_stage0.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6AD000-1F21-4474-A5B1-DA4132FB08BD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B44D1A1-6E83-4AFB-A3DD-8622737AFC28}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="14805" windowHeight="7650" tabRatio="868" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="10" r:id="rId1"/>
@@ -423,7 +423,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="305">
   <si>
     <t>Name</t>
   </si>
@@ -1336,6 +1336,12 @@
   </si>
   <si>
     <t>Nothing here since controlled through test scripts</t>
+  </si>
+  <si>
+    <t>Corduff 110 kV</t>
+  </si>
+  <si>
+    <t>110 kV B1</t>
   </si>
 </sst>
 </file>
@@ -2149,7 +2155,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -6231,8 +6237,8 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6304,10 +6310,18 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D8" s="3" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -9707,6 +9721,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <iab7cdb7554d4997ae876b11632fa575 xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca">
@@ -9715,15 +9738,6 @@
     <TaxCatchAll xmlns="3cada6dc-2705-46ed-bab2-0b2cd6d935ca"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9745,6 +9759,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FCC61AA8-C35E-4598-8617-08B80F018AC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -9758,12 +9780,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B5D7682-109C-47ED-9D9D-D061E76CCAD3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>